<commit_message>
Adding Excel file to repository
</commit_message>
<xml_diff>
--- a/Data/List_Generator.xlsx
+++ b/Data/List_Generator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\Python Scripts\Pandas_for_work\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA52ECFC-1BEF-4625-85A5-11D0691346AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD58C58-9A62-488D-BE4D-90846A527F27}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="420" windowWidth="19995" windowHeight="8850" xr2:uid="{AF62C369-36C7-4C27-8816-4A4745CBCA71}"/>
+    <workbookView xWindow="360" yWindow="420" windowWidth="19995" windowHeight="10755" activeTab="3" xr2:uid="{AF62C369-36C7-4C27-8816-4A4745CBCA71}"/>
   </bookViews>
   <sheets>
     <sheet name="B" sheetId="1" r:id="rId1"/>
@@ -414,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF1A2B4-0D02-4B90-8099-F3061796E668}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -431,7 +431,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <f ca="1">RANDBETWEEN(1,101)</f>
-        <v>94</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -440,7 +440,7 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A66" ca="1" si="0">RANDBETWEEN(1,101)</f>
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -449,7 +449,7 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -458,7 +458,7 @@
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="C5">
         <v>6</v>
@@ -467,7 +467,7 @@
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -476,7 +476,7 @@
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C7">
         <v>11</v>
@@ -485,7 +485,7 @@
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C8">
         <v>13</v>
@@ -494,7 +494,7 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C9">
         <v>14</v>
@@ -503,7 +503,7 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="C10">
         <v>15</v>
@@ -512,7 +512,7 @@
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="C11">
         <v>17</v>
@@ -521,7 +521,7 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C12">
         <v>18</v>
@@ -530,7 +530,7 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="C13">
         <v>22</v>
@@ -539,7 +539,7 @@
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C14">
         <v>23</v>
@@ -548,7 +548,7 @@
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C15">
         <v>25</v>
@@ -557,7 +557,7 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="C16">
         <v>26</v>
@@ -566,7 +566,7 @@
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <v>27</v>
@@ -575,7 +575,7 @@
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>29</v>
@@ -584,7 +584,7 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C19">
         <v>30</v>
@@ -593,7 +593,7 @@
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="C20">
         <v>31</v>
@@ -602,7 +602,7 @@
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="C21">
         <v>33</v>
@@ -611,7 +611,7 @@
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="C22">
         <v>34</v>
@@ -620,7 +620,7 @@
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="C23">
         <v>35</v>
@@ -629,7 +629,7 @@
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C24">
         <v>37</v>
@@ -638,7 +638,7 @@
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>14</v>
       </c>
       <c r="C25">
         <v>38</v>
@@ -647,7 +647,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C26">
         <v>39</v>
@@ -656,7 +656,7 @@
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="C27">
         <v>40</v>
@@ -665,7 +665,7 @@
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="C28">
         <v>41</v>
@@ -674,7 +674,7 @@
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="C29">
         <v>42</v>
@@ -683,7 +683,7 @@
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="C30">
         <v>44</v>
@@ -692,7 +692,7 @@
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C31">
         <v>45</v>
@@ -701,7 +701,7 @@
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C32">
         <v>46</v>
@@ -710,7 +710,7 @@
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="C33">
         <v>49</v>
@@ -719,7 +719,7 @@
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="C34">
         <v>50</v>
@@ -728,7 +728,7 @@
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="C35">
         <v>55</v>
@@ -737,7 +737,7 @@
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="C36">
         <v>56</v>
@@ -746,7 +746,7 @@
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="C37">
         <v>57</v>
@@ -755,7 +755,7 @@
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="C38">
         <v>58</v>
@@ -764,7 +764,7 @@
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="C39">
         <v>59</v>
@@ -773,7 +773,7 @@
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C40">
         <v>60</v>
@@ -782,7 +782,7 @@
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C41">
         <v>61</v>
@@ -791,7 +791,7 @@
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C42">
         <v>62</v>
@@ -800,7 +800,7 @@
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C43">
         <v>64</v>
@@ -809,7 +809,7 @@
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C44">
         <v>65</v>
@@ -818,7 +818,7 @@
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" ca="1" si="0"/>
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="C45">
         <v>67</v>
@@ -827,7 +827,7 @@
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="C46">
         <v>68</v>
@@ -836,7 +836,7 @@
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C47">
         <v>71</v>
@@ -845,7 +845,7 @@
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" ca="1" si="0"/>
-        <v>101</v>
+        <v>55</v>
       </c>
       <c r="C48">
         <v>72</v>
@@ -854,7 +854,7 @@
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="C49">
         <v>76</v>
@@ -863,7 +863,7 @@
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="C50">
         <v>77</v>
@@ -872,7 +872,7 @@
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="C51">
         <v>79</v>
@@ -881,7 +881,7 @@
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C52">
         <v>80</v>
@@ -890,7 +890,7 @@
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="C53">
         <v>82</v>
@@ -899,7 +899,7 @@
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="C54">
         <v>84</v>
@@ -908,7 +908,7 @@
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C55">
         <v>86</v>
@@ -917,7 +917,7 @@
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="C56">
         <v>87</v>
@@ -926,7 +926,7 @@
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>8</v>
       </c>
       <c r="C57">
         <v>89</v>
@@ -935,7 +935,7 @@
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C58">
         <v>91</v>
@@ -944,7 +944,7 @@
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="C59">
         <v>92</v>
@@ -953,7 +953,7 @@
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C60">
         <v>93</v>
@@ -962,7 +962,7 @@
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C61">
         <v>94</v>
@@ -971,7 +971,7 @@
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="C62">
         <v>95</v>
@@ -980,7 +980,7 @@
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="C63">
         <v>97</v>
@@ -989,7 +989,7 @@
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="C64">
         <v>99</v>
@@ -1007,7 +1007,7 @@
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C66">
         <v>101</v>
@@ -1016,211 +1016,211 @@
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" ref="A67:A101" ca="1" si="1">RANDBETWEEN(1,101)</f>
-        <v>89</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>88</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>80</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" ca="1" si="1"/>
-        <v>41</v>
+        <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" ca="1" si="1"/>
-        <v>92</v>
+        <v>42</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>61</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" ca="1" si="1"/>
-        <v>68</v>
+        <v>51</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" ca="1" si="1"/>
-        <v>44</v>
+        <v>75</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>40</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>68</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>96</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" ca="1" si="1"/>
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" ca="1" si="1"/>
-        <v>83</v>
+        <v>29</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" ca="1" si="1"/>
-        <v>49</v>
+        <v>82</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>81</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <v>53</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <v>71</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" ca="1" si="1"/>
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>38</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" ca="1" si="1"/>
-        <v>99</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>66</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101">
         <f t="shared" ca="1" si="1"/>
-        <v>57</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1972,7 +1972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B3CFEF-2B9C-42E3-8F2E-DA8EF949B860}">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -3008,6 +3008,8 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:A76">
     <sortCondition ref="A3:A76"/>
   </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="1" gridLines="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>